<commit_message>
I performed two operations over git
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Git Checklist" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="176">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -538,6 +538,18 @@
   </si>
   <si>
     <t xml:space="preserve">GIT Resolving Conflict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT stash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store uncompleted work on remote repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push to a remote branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push and pull to a remote branch</t>
   </si>
 </sst>
 </file>
@@ -547,7 +559,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -571,6 +583,13 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
@@ -639,7 +658,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -664,6 +683,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,7 +699,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -767,8 +790,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -800,93 +823,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3"/>
@@ -894,75 +917,75 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -974,7 +997,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -986,7 +1009,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -998,7 +1021,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1010,7 +1033,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1022,7 +1045,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1034,7 +1057,7 @@
         <v>41</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1046,7 +1069,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1058,7 +1081,7 @@
         <v>45</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1070,7 +1093,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1081,7 +1104,7 @@
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,15 +1114,15 @@
       <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,7 +1132,7 @@
       <c r="B29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,7 +1142,7 @@
       <c r="B30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1152,7 @@
       <c r="B31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1162,7 @@
       <c r="B32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1172,7 @@
       <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,7 +1182,7 @@
       <c r="B34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,7 +1192,7 @@
       <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,7 +1202,7 @@
       <c r="B36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,7 +1212,7 @@
       <c r="B37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="6"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1222,7 @@
       <c r="B38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,7 +1232,7 @@
       <c r="B39" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,7 +1242,7 @@
       <c r="B40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,7 +1252,7 @@
       <c r="B41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1262,7 @@
       <c r="B42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1272,7 @@
       <c r="B43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="6"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1259,7 +1282,7 @@
       <c r="B44" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="2"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1347,7 +1370,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1359,10 +1382,10 @@
         <v>72</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1374,7 +1397,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1386,7 +1409,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1398,7 +1421,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1410,7 +1433,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1422,7 +1445,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1434,7 +1457,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1446,7 +1469,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1458,7 +1481,7 @@
         <v>89</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1470,7 +1493,7 @@
         <v>91</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1482,7 +1505,7 @@
         <v>93</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1494,7 +1517,7 @@
         <v>95</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1506,7 +1529,7 @@
         <v>97</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1518,7 +1541,7 @@
         <v>99</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1530,7 +1553,7 @@
         <v>101</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1542,7 +1565,7 @@
         <v>103</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1554,7 +1577,7 @@
         <v>105</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1566,7 +1589,7 @@
         <v>107</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1578,7 +1601,7 @@
         <v>109</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1590,7 +1613,7 @@
         <v>111</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="10" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1602,7 +1625,7 @@
         <v>113</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="10" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1614,7 +1637,7 @@
         <v>115</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1626,7 +1649,7 @@
         <v>117</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1638,7 +1661,7 @@
         <v>119</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1650,7 +1673,7 @@
         <v>121</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1662,7 +1685,7 @@
         <v>123</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1674,7 +1697,7 @@
         <v>125</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1686,7 +1709,7 @@
         <v>127</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1698,79 +1721,79 @@
         <v>129</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="10" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="3"/>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="3"/>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="3"/>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3"/>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="3"/>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="3"/>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="3"/>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="3"/>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="3"/>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="3"/>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="3"/>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="3"/>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="10" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1779,7 +1802,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="3"/>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="10" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1846,15 +1869,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.61"/>
@@ -1876,7 +1899,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -1887,7 +1910,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -1901,7 +1924,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -1912,7 +1935,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -1923,7 +1946,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="11" t="n">
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -1934,7 +1957,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -1945,18 +1968,18 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="11" t="n">
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -1967,7 +1990,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="11" t="n">
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -1978,7 +2001,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="11" t="n">
         <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -1989,7 +2012,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="11" t="n">
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -2000,7 +2023,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="11" t="n">
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -2011,7 +2034,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="11" t="n">
         <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -2019,6 +2042,28 @@
       </c>
       <c r="C14" s="0" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2036,6 +2081,8 @@
     <hyperlink ref="C12" r:id="rId11" display="GIT Branch Various Commands"/>
     <hyperlink ref="C13" r:id="rId12" display="GIT Difference Commands"/>
     <hyperlink ref="C14" r:id="rId13" display="GIT Resolving Conflict"/>
+    <hyperlink ref="C15" r:id="rId14" display="Store uncompleted work on remote repository"/>
+    <hyperlink ref="C16" r:id="rId15" display="Push and pull to a remote branch"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>